<commit_message>
AgeCalc programs changed for cups/corals
</commit_message>
<xml_diff>
--- a/empty_chemblank.xlsx
+++ b/empty_chemblank.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julianissen/Desktop/Up to date blank spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julianissen/Isotope_Lab_Programs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -485,7 +485,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -540,19 +540,19 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -560,19 +560,19 @@
         <v>11</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>